<commit_message>
Implemented new way of specifying flags. Added test cases.
</commit_message>
<xml_diff>
--- a/test/assets/test.xlsx
+++ b/test/assets/test.xlsx
@@ -82,22 +82,22 @@
     <t xml:space="preserve">hello.png</t>
   </si>
   <si>
-    <t xml:space="preserve">phrase (en)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phrase (pl)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phrase (ua)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">picture (en, import)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">picture (pl, import)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">picture (ua, import)</t>
+    <t xml:space="preserve">phrase (EN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phrase (PL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phrase (UA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picture (EN, IMPORT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picture (PL, IMPORT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picture (UA, IMPORT)</t>
   </si>
   <si>
     <t xml:space="preserve">Hello</t>
@@ -362,7 +362,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,7 +423,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="16.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.51"/>
   </cols>
   <sheetData>

</xml_diff>